<commit_message>
Now we must enter specifics, but it makes it to where we can use it with any sheet
</commit_message>
<xml_diff>
--- a/Resources/Population_From_2019_2023.xlsx
+++ b/Resources/Population_From_2019_2023.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="49" documentId="11_96766634C2220C87399AF1ADC61CE69448D2ADC7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E852C22-DFCA-491B-8CFD-30AEB938AA58}"/>
   <bookViews>
-    <workbookView xWindow="10335" yWindow="975" windowWidth="11265" windowHeight="9308" firstSheet="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10335" yWindow="975" windowWidth="11265" windowHeight="9308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population" sheetId="1" r:id="rId1"/>
@@ -351,8 +351,8 @@
   </sheetPr>
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>